<commit_message>
Criando o arquivo de explicação
</commit_message>
<xml_diff>
--- a/Usuarios.xlsx
+++ b/Usuarios.xlsx
@@ -641,12 +641,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>If they had saved more money, they would be in a better financial situation now.</t>
+          <t>If he had pursued his passion, he might be happier now.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Se tivessem economizado mais dinheiro, estariam em uma situação financeira melhor agora.</t>
+          <t>Se tivesse seguido sua paixão, poderia estar mais feliz agora.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -661,12 +661,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>If they had known about the sale, they would have bought more.</t>
+          <t>She wishes she had traveled more before starting a family.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Se eles tivessem sabido da liquidação, eles teriam comprado mais.</t>
+          <t>Ela gostaria de ter viajado mais antes de começar uma família.</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">

</xml_diff>

<commit_message>
Add bot interface and section 'Aprender'
</commit_message>
<xml_diff>
--- a/Usuarios.xlsx
+++ b/Usuarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faell\OneDrive\Documentos\GitHub\EnglishBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0722C2-213F-46A3-83BE-EBBDC9F91E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED4C9A5-B1BE-4867-8C3C-515ABFAB5081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23445" yWindow="240" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>id</t>
   </si>
@@ -34,22 +34,13 @@
     <t>nivel</t>
   </si>
   <si>
-    <t>45678</t>
-  </si>
-  <si>
-    <t>usuario novo</t>
-  </si>
-  <si>
-    <t>Que horas são?</t>
-  </si>
-  <si>
-    <t>Basico</t>
-  </si>
-  <si>
-    <t>356</t>
-  </si>
-  <si>
-    <t>What time is it?</t>
+    <t>number</t>
+  </si>
+  <si>
+    <t>ultima mensagem</t>
+  </si>
+  <si>
+    <t>Frases  / Aprender</t>
   </si>
 </sst>
 </file>
@@ -424,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,9 +427,12 @@
     <col min="2" max="2" width="40.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="86" style="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="61.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,89 +445,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update - add user class in app.py and CodigoDocumentado.ipynb
</commit_message>
<xml_diff>
--- a/Usuarios.xlsx
+++ b/Usuarios.xlsx
@@ -1,64 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\faell\OneDrive\Documentos\GitHub\EnglishBot\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED4C9A5-B1BE-4867-8C3C-515ABFAB5081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23445" yWindow="240" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>frase</t>
-  </si>
-  <si>
-    <t>traducao</t>
-  </si>
-  <si>
-    <t>nivel</t>
-  </si>
-  <si>
-    <t>number</t>
-  </si>
-  <si>
-    <t>ultima mensagem</t>
-  </si>
-  <si>
-    <t>Frases  / Aprender</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -77,24 +46,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -414,48 +442,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="86" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="61.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col width="23.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="40.42578125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="86" customWidth="1" style="1" min="3" max="3"/>
+    <col width="30.28515625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="15.5703125" customWidth="1" min="5" max="5"/>
+    <col width="61.5703125" customWidth="1" min="6" max="6"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>frase</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>traducao</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>nivel</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>number</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ultima comando</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Frases  / Aprender</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1972887851</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>If they had finished their work earlier, they could have gone to the party.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Se eles tivessem terminado o trabalho mais cedo, eles poderiam ter ido à festa.</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Intermediário</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>86</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>/OK</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Frase</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.787401575" bottom="0.787401575" header="0.31496062" footer="0.31496062"/>
 </worksheet>
 </file>
</xml_diff>